<commit_message>
updated task facet notes based on the TREC topics. prioritized which ones I will implement for now
</commit_message>
<xml_diff>
--- a/taskfacets.xlsx
+++ b/taskfacets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmsch\Desktop\COVIDsearch\covid\taskmodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmsch\Desktop\COVIDsearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF5A038-D74E-4C17-B2D1-FB14571575C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AD4F48-D239-44B2-BDBB-C9B6A6466CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D75EA5-E379-4D8D-B7BC-20CF8BE02458}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="177">
   <si>
     <t>facet 1) level: individual/group/environment</t>
   </si>
@@ -396,9 +397,6 @@
     <t>severe</t>
   </si>
   <si>
-    <t>unsevere/regular/any</t>
-  </si>
-  <si>
     <t>how do people die from the coronaviru</t>
   </si>
   <si>
@@ -420,10 +418,151 @@
     <t>coronavirus under reporting</t>
   </si>
   <si>
-    <t>kijk kTask1</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>coronavirus in Canada</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>coronavirus social distancing impact</t>
+  </si>
+  <si>
+    <t>bedoel ik realtime of publication time</t>
+  </si>
+  <si>
+    <t>coronavirus hospital rationing</t>
+  </si>
+  <si>
+    <t>coronavirus quarantine</t>
+  </si>
+  <si>
+    <t>infected</t>
+  </si>
+  <si>
+    <t>uninfected</t>
+  </si>
+  <si>
+    <t>severe infection</t>
+  </si>
+  <si>
+    <t>unaffected</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>how does coronavirus spread</t>
+  </si>
+  <si>
+    <t>coronavirus super spreaders</t>
+  </si>
+  <si>
+    <t>historical</t>
+  </si>
+  <si>
+    <t>prevent</t>
+  </si>
+  <si>
+    <t>coronavirus outside body</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>how long does coronavirus survive on surfaces</t>
+  </si>
+  <si>
+    <t>coronavirus clinical trials</t>
+  </si>
+  <si>
+    <t>masks prevent coronavirus</t>
+  </si>
+  <si>
+    <t>what alcohol sanitizer kills coronavirus</t>
+  </si>
+  <si>
+    <t>coronavirus and ACE inhibitors</t>
+  </si>
+  <si>
+    <t>coronavirus mortality</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>coronavirus heart impacts</t>
+  </si>
+  <si>
+    <t>easiest way: use the medical dictionary to get terms for each facet (where it is applicable)</t>
+  </si>
+  <si>
+    <t>then use thematic tagger approach to tag all</t>
+  </si>
+  <si>
+    <t>host/virus</t>
+  </si>
+  <si>
+    <t>coronavirus hypertension</t>
+  </si>
+  <si>
+    <t>high-risk groups</t>
+  </si>
+  <si>
+    <t>overlap the two risks</t>
+  </si>
+  <si>
+    <t>coronavirus diabetes</t>
+  </si>
+  <si>
+    <t>coronavirus biomarkers</t>
+  </si>
+  <si>
+    <t>coronavirus early symptom</t>
+  </si>
+  <si>
+    <t>diagnostic</t>
+  </si>
+  <si>
+    <t>coronavirus asymptomatic</t>
+  </si>
+  <si>
+    <t>coronavirus hydroxychloroquine</t>
+  </si>
+  <si>
+    <t>coronavirus drug repurposing</t>
+  </si>
+  <si>
+    <t>coronavirus remdesivir</t>
+  </si>
+  <si>
+    <t>transmission, incubation, environment</t>
+  </si>
+  <si>
+    <t>virus genetics, origin, evolution</t>
+  </si>
+  <si>
+    <t>vaccines, therapeutics</t>
+  </si>
+  <si>
+    <t>medical care</t>
+  </si>
+  <si>
+    <t>non-pharmaceutical interventions</t>
+  </si>
+  <si>
+    <t>geography and virality (epidemiology)</t>
+  </si>
+  <si>
+    <t>diagnostics, surveillance</t>
+  </si>
+  <si>
+    <t>ethical and social science</t>
+  </si>
+  <si>
+    <t>information sharing, inter-sectoral collaboration</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -842,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A346B5-4FDE-4F61-8BE3-F28FE97BCCD2}">
-  <dimension ref="A1:Y52"/>
+  <dimension ref="A1:BC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,7 +994,7 @@
     <col min="9" max="9" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,16 +1004,22 @@
       <c r="R1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AO1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AH2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -882,8 +1027,14 @@
         <v>112</v>
       </c>
       <c r="Q3" s="4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AA3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -906,22 +1057,88 @@
         <v>119</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="X5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AA5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -967,8 +1184,80 @@
       <c r="Y6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -990,9 +1279,6 @@
       <c r="J7" t="s">
         <v>53</v>
       </c>
-      <c r="O7" t="s">
-        <v>116</v>
-      </c>
       <c r="P7" t="s">
         <v>66</v>
       </c>
@@ -1020,8 +1306,86 @@
       <c r="Y7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1050,7 +1414,7 @@
         <v>60</v>
       </c>
       <c r="N8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P8" t="s">
         <v>67</v>
@@ -1079,8 +1443,89 @@
       <c r="Y8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1129,13 +1574,88 @@
       <c r="Y9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1678,7 @@
         <v>52</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="P11" t="s">
         <v>117</v>
@@ -1187,8 +1707,89 @@
       <c r="Y11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>81</v>
       </c>
@@ -1220,7 +1821,7 @@
         <v>99</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="P12" t="s">
         <v>117</v>
@@ -1238,7 +1839,7 @@
         <v>82</v>
       </c>
       <c r="V12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W12" t="s">
         <v>74</v>
@@ -1249,13 +1850,94 @@
       <c r="Y12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1304,8 +1986,83 @@
       <c r="Y14" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1327,6 +2084,9 @@
       <c r="J15" t="s">
         <v>101</v>
       </c>
+      <c r="O15" t="s">
+        <v>116</v>
+      </c>
       <c r="P15" t="s">
         <v>66</v>
       </c>
@@ -1354,8 +2114,83 @@
       <c r="Y15" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1383,6 +2218,9 @@
       <c r="L16" t="s">
         <v>92</v>
       </c>
+      <c r="O16" t="s">
+        <v>116</v>
+      </c>
       <c r="P16" t="s">
         <v>103</v>
       </c>
@@ -1410,8 +2248,92 @@
       <c r="Y16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>98</v>
       </c>
@@ -1422,10 +2344,19 @@
         <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="I17" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+      <c r="J17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" t="s">
+        <v>138</v>
+      </c>
+      <c r="O17" t="s">
+        <v>176</v>
       </c>
       <c r="P17" t="s">
         <v>107</v>
@@ -1437,61 +2368,261 @@
         <v>116</v>
       </c>
       <c r="T17" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="U17" t="s">
         <v>120</v>
       </c>
       <c r="V17" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="W17" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="X17" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="Y17" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>135</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>8</v>
+      </c>
+      <c r="N19" t="s">
+        <v>167</v>
+      </c>
+      <c r="S19" t="s">
+        <v>116</v>
+      </c>
+      <c r="U19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>168</v>
+      </c>
+      <c r="R21" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22" t="s">
+        <v>169</v>
+      </c>
+      <c r="T22" t="s">
+        <v>116</v>
+      </c>
+      <c r="V22" t="s">
+        <v>116</v>
+      </c>
+      <c r="X22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
@@ -1501,24 +2632,66 @@
       <c r="C25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>5</v>
+      </c>
+      <c r="N26" t="s">
+        <v>173</v>
+      </c>
+      <c r="W26" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>174</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1528,13 +2701,19 @@
       <c r="C28" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -1542,7 +2721,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
bm25 run and reranking run (near finished)
</commit_message>
<xml_diff>
--- a/taskfacets.xlsx
+++ b/taskfacets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmsch\Desktop\COVIDsearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AD4F48-D239-44B2-BDBB-C9B6A6466CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DB25D9-4D64-47AC-9445-0D4530C6CDE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D75EA5-E379-4D8D-B7BC-20CF8BE02458}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="177">
   <si>
     <t>facet 1) level: individual/group/environment</t>
   </si>
@@ -983,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A346B5-4FDE-4F61-8BE3-F28FE97BCCD2}">
   <dimension ref="A1:BC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AS22" sqref="AS22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2479,29 +2478,29 @@
       <c r="N19" t="s">
         <v>167</v>
       </c>
-      <c r="S19" t="s">
-        <v>116</v>
-      </c>
-      <c r="U19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>116</v>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
       </c>
       <c r="AW19" t="s">
         <v>167</v>
@@ -2517,17 +2516,17 @@
       <c r="N20" t="s">
         <v>86</v>
       </c>
-      <c r="AK20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>116</v>
+      <c r="AK20">
+        <v>1</v>
+      </c>
+      <c r="AN20">
+        <v>1</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20">
+        <v>1</v>
       </c>
       <c r="AW20" t="s">
         <v>86</v>
@@ -2543,8 +2542,8 @@
       <c r="N21" t="s">
         <v>168</v>
       </c>
-      <c r="R21" t="s">
-        <v>116</v>
+      <c r="R21">
+        <v>2</v>
       </c>
       <c r="AW21" t="s">
         <v>168</v>
@@ -2560,23 +2559,23 @@
       <c r="N22" t="s">
         <v>169</v>
       </c>
-      <c r="T22" t="s">
-        <v>116</v>
-      </c>
-      <c r="V22" t="s">
-        <v>116</v>
-      </c>
-      <c r="X22" t="s">
-        <v>116</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT22" t="s">
-        <v>116</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>116</v>
+      <c r="T22">
+        <v>3</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="X22">
+        <v>3</v>
+      </c>
+      <c r="AS22">
+        <v>3</v>
+      </c>
+      <c r="AT22">
+        <v>3</v>
+      </c>
+      <c r="AU22">
+        <v>3</v>
       </c>
       <c r="AW22" t="s">
         <v>169</v>
@@ -2592,8 +2591,8 @@
       <c r="N23" t="s">
         <v>170</v>
       </c>
-      <c r="AB23" t="s">
-        <v>116</v>
+      <c r="AB23">
+        <v>4</v>
       </c>
       <c r="AW23" t="s">
         <v>170</v>
@@ -2606,17 +2605,17 @@
       <c r="N24" t="s">
         <v>171</v>
       </c>
-      <c r="AA24" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>116</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>116</v>
+      <c r="AA24">
+        <v>5</v>
+      </c>
+      <c r="AC24">
+        <v>5</v>
+      </c>
+      <c r="AI24">
+        <v>5</v>
+      </c>
+      <c r="AJ24">
+        <v>5</v>
       </c>
       <c r="AW24" t="s">
         <v>171</v>
@@ -2638,8 +2637,8 @@
       <c r="N25" t="s">
         <v>172</v>
       </c>
-      <c r="Z25" t="s">
-        <v>116</v>
+      <c r="Z25">
+        <v>6</v>
       </c>
       <c r="AW25" t="s">
         <v>172</v>
@@ -2658,20 +2657,20 @@
       <c r="N26" t="s">
         <v>173</v>
       </c>
-      <c r="W26" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>116</v>
-      </c>
-      <c r="AR26" t="s">
-        <v>116</v>
+      <c r="W26">
+        <v>7</v>
+      </c>
+      <c r="Y26">
+        <v>7</v>
+      </c>
+      <c r="AH26">
+        <v>7</v>
+      </c>
+      <c r="AQ26">
+        <v>7</v>
+      </c>
+      <c r="AR26">
+        <v>7</v>
       </c>
       <c r="AW26" t="s">
         <v>173</v>

</xml_diff>